<commit_message>
Finish the prototype dfu Update main program to adjust dfu classroom programming update classroom
</commit_message>
<xml_diff>
--- a/微信摇一摇教室.xlsx
+++ b/微信摇一摇教室.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="自己" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>7A403</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>7A114</t>
+  </si>
+  <si>
+    <t>7A104</t>
+  </si>
+  <si>
+    <t>7A215</t>
   </si>
 </sst>
 </file>
@@ -374,84 +380,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>21931</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="str">
+        <f>DEC2HEX(B1)</f>
+        <v>55AB</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>22047</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C9" si="0">DEC2HEX(B2)</f>
+        <v>561F</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>21933</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>55AD</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>21935</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>55AF</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>21926</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>55A6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>22103</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>22104</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <v>21920</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>55A0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
         <v>21917</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>559D</v>
       </c>
     </row>
   </sheetData>
@@ -461,20 +503,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1">
         <v>21896</v>
+      </c>
+      <c r="C1" t="str">
+        <f>DEC2HEX(B1)</f>
+        <v>5588</v>
       </c>
     </row>
   </sheetData>
@@ -484,39 +530,88 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1">
         <v>21889</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="str">
+        <f>DEC2HEX(B1)</f>
+        <v>5581</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <v>21926</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C3" si="0">DEC2HEX(B2)</f>
+        <v>55A6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
         <v>21975</v>
       </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>55D7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>21896</v>
+      </c>
+      <c r="C4" t="str">
+        <f>DEC2HEX(B4)</f>
+        <v>5588</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>21888</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" ref="C5:C6" si="1">DEC2HEX(B5)</f>
+        <v>5580</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>21911</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>5597</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>